<commit_message>
20180731 15:04 revised abc.xlsx
</commit_message>
<xml_diff>
--- a/abc.xlsx
+++ b/abc.xlsx
@@ -16,9 +16,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>now 2018-7-31 15Pm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">now </t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -65,8 +69,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -363,17 +373,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="E2"/>
+  <dimension ref="E2:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
+  <cols>
+    <col min="6" max="6" width="10.26953125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="5:5">
+    <row r="2" spans="5:7">
       <c r="E2" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="5:7">
+      <c r="E4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2">
+        <v>43312</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.62777777777777777</v>
       </c>
     </row>
   </sheetData>

</xml_diff>